<commit_message>
Added No Text CSV
</commit_message>
<xml_diff>
--- a/resources/features.xlsx
+++ b/resources/features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessedecker/Mercyhurst/CIS_572/final/tw_net/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08127D3-4B80-B04A-98BF-19A4BFF5A656}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9077052-A10C-AC4A-A9CA-8F1386CB8F96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{8734DA11-6BEB-3942-8FF0-422E43E44FD2}"/>
+    <workbookView xWindow="10280" yWindow="3880" windowWidth="30620" windowHeight="18860" activeTab="3" xr2:uid="{8734DA11-6BEB-3942-8FF0-422E43E44FD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Determine Unluence" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="159">
   <si>
     <t>created_at</t>
   </si>
@@ -444,9 +444,6 @@
     <t xml:space="preserve">isVerified </t>
   </si>
   <si>
-    <t xml:space="preserve">isRetweeted </t>
-  </si>
-  <si>
     <t>1 to 7</t>
   </si>
   <si>
@@ -465,13 +462,49 @@
     <t>category</t>
   </si>
   <si>
-    <t>Remove - None are retweets</t>
-  </si>
-  <si>
     <t>Sunday = 1</t>
   </si>
   <si>
     <t>Midnight = 0</t>
+  </si>
+  <si>
+    <t>Number of years the user has been active</t>
+  </si>
+  <si>
+    <t>1 = the tweet is a reply to another tweet</t>
+  </si>
+  <si>
+    <t>1 = the user is verified</t>
+  </si>
+  <si>
+    <t>number retweets</t>
+  </si>
+  <si>
+    <t>number favorites</t>
+  </si>
+  <si>
+    <t>number hashtags in tweet</t>
+  </si>
+  <si>
+    <t>number symbols in tweet</t>
+  </si>
+  <si>
+    <t>number media in tweet</t>
+  </si>
+  <si>
+    <t>number urls in tweet</t>
+  </si>
+  <si>
+    <t>number users mentioned in tweet</t>
+  </si>
+  <si>
+    <t>each interval = 2 hrs. add to created_hr to find time of day</t>
+  </si>
+  <si>
+    <t>isRetweeted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 = the tweet has been retweeted </t>
   </si>
 </sst>
 </file>
@@ -1309,7 +1342,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2126,11 +2159,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA933A2F-0678-7947-A704-1A1C4472C7DF}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2138,7 +2171,7 @@
     <col min="1" max="1" width="66.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="4" max="4" width="58.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2160,10 +2193,13 @@
         <v>130</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2171,13 +2207,13 @@
         <v>119</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2185,13 +2221,13 @@
         <v>135</v>
       </c>
       <c r="B4" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
         <v>144</v>
-      </c>
-      <c r="C4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2202,7 +2238,10 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="D5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2213,7 +2252,10 @@
         <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="D6" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2224,7 +2266,10 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="D7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2235,7 +2280,10 @@
         <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2246,43 +2294,52 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>138</v>
+      <c r="A10" t="s">
+        <v>137</v>
       </c>
       <c r="B10" t="s">
         <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
         <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="D11" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
         <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="D12" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2293,35 +2350,66 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="D13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>141</v>
+      </c>
+      <c r="D14" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>132</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>